<commit_message>
Update Runway and Cash Budget Tool Foresight v1.2.xlsx
</commit_message>
<xml_diff>
--- a/Runway and Cash Budget Tool Foresight v1.2.xlsx
+++ b/Runway and Cash Budget Tool Foresight v1.2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1120" yWindow="1120" windowWidth="24480" windowHeight="14940" tabRatio="500"/>
+    <workbookView xWindow="30980" yWindow="3120" windowWidth="25500" windowHeight="15700" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="11" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <sheet name="Changelog" sheetId="18" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">README!$B$2:$B$44</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">README!$B$2:$B$45</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="331">
   <si>
     <t>Year</t>
   </si>
@@ -580,16 +580,7 @@
     <t>License</t>
   </si>
   <si>
-    <t>Subject to your compliance with these Terms, you are hereby granted a non-exclusive, limited, non-transferable, revocable license to use the Product as we intend for them to be used. This license applies to a single individual or company, and may not be distributed for reuse outside of yourself or your company. You are licensed to keep, for your own personal records, electronic or physical copies of documents you have created from the Product. You may not copy the content of the models for use or sale. Any rights not expressly granted in these Terms are reserved by us.</t>
-  </si>
-  <si>
-    <t>Resale or unauthorized distribution of materials downloaded from the website is strictly prohibited. Use of these materials is for your personal or business use. Any resale or redistribution of our materials requires express written consent from us.</t>
-  </si>
-  <si>
     <t>Intellectual Property Rights</t>
-  </si>
-  <si>
-    <t>We retain all right, title and interest in and to the products, including, without limitation, software, images, text, graphics, illustrations, logos, service marks, copyrights, photographs, videos, music, spreadsheet methods, and all related intellectual property rights. Except as otherwise provided in this agreement, you may not, and may not permit others to: (i) reproduce, modify, translate, enhance, decompile, disassemble, reverse engineer or create derivative works of any of our Product; (ii) sell, license, sublicense, rent, lease, distribute, copy, publicly display, publish, adapt or edit any of our Product; or (iii) circumvent or disable any security or technological features of our Product.</t>
   </si>
   <si>
     <t>The design, text, graphics, selection and arrangement thereof and services and the legal forms, documents, guidance and all other content found on our website are the copyright © of us. All rights reserved.</t>
@@ -946,9 +937,6 @@
     <t>Use of this model signifies acceptance of terms of use.</t>
   </si>
   <si>
-    <t>The license is summarized in the terms or use below, and in detail at https://foresight.is/terms</t>
-  </si>
-  <si>
     <t>Visit https://foresight.is/learn/runway-cash-budget-overview to get more instructions and videos on how to use the model, including details on each sheet and key components.</t>
   </si>
   <si>
@@ -1003,9 +991,6 @@
     <t>4) Traction &amp; Ownership: A summary that compares cash on hand to ownership (founders, common shareholders) to a traction metric. This traction metric can be revenues, or some other metric input into the model by the user.</t>
   </si>
   <si>
-    <t>Completely new version that is based off a streamlined Starter Model (https://foresight.is/starter-financial-model). This includes a couple new features on costs and summary, but is largely the same as v1.2.</t>
-  </si>
-  <si>
     <t>v1.2 - 15 January 2019</t>
   </si>
   <si>
@@ -1016,6 +1001,27 @@
   </si>
   <si>
     <t>Standard Model:https://foresight.is/learn/runway-cash-budget-overview</t>
+  </si>
+  <si>
+    <t>Completely new version that is based off a streamlined Starter Model (https://foresight.is/starter-financial-model). This includes a couple new features on costs and summary, but is largely the same as v1.1.</t>
+  </si>
+  <si>
+    <t>Full license details at https://creativecommons.org/licenses/by-nc-sa/4.0/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is licensed under a Creative Commons Attribution-NonCommercial-ShareAlike 4.0 International license. You are free to a) Share — copy and redistribute the material in any medium or format, and b) Adapt — remix, transform, and build upon the material. Under the following terms of c) Attribution — You must give appropriate credit, provide a link to the license, and indicate if changes were made. You may do so in any reasonable manner, but not in any way that suggests the licensor endorses you or your use, d) NonCommercial — You may not use the material for commercial purposes, and e) ShareAlike — If you remix, transform, or build upon the material, you must distribute your contributions under the same license as the original. Full license details are at https://creativecommons.org/licenses/by-nc-sa/4.0/ </t>
+  </si>
+  <si>
+    <t>This is licensed under Creative Commons Attribution-NonCommercial-ShareAlike 4.0 International</t>
+  </si>
+  <si>
+    <t>Updated license terms to a Creative Commons license. See more on Github: https://github.com/foresighthq/runway-tool/</t>
+  </si>
+  <si>
+    <t>We retain all right, title and interest in, without limitation, graphics, illustrations, logos, service marks, copyrights, photographs, videos, formulas, spreadsheet methods, and text, and all related intellectual property rights.</t>
+  </si>
+  <si>
+    <t>Contributions from third-parties that are accepted into the template are owned by Unstructured Ventures, LLC, and Unstructured Ventures owns all rights to commercial use and patents. Any rights not expressly granted in these Terms are reserved by us.</t>
   </si>
 </sst>
 </file>
@@ -1327,7 +1333,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1102">
+  <cellStyleXfs count="1103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2419,6 +2425,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2710,7 +2717,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1102">
+  <cellStyles count="1103">
     <cellStyle name="amount" xfId="5"/>
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Comma 10" xfId="6"/>
@@ -3604,6 +3611,7 @@
     <cellStyle name="Followed Hyperlink" xfId="1099" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1100" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1101" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1102" builtinId="9" hidden="1"/>
     <cellStyle name="header" xfId="53"/>
     <cellStyle name="Header Total" xfId="54"/>
     <cellStyle name="Header1" xfId="55"/>
@@ -4281,11 +4289,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="100"/>
-        <c:axId val="-2065148184"/>
-        <c:axId val="2136513240"/>
+        <c:axId val="-2118817192"/>
+        <c:axId val="-2118373112"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2065148184"/>
+        <c:axId val="-2118817192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4295,7 +4303,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2136513240"/>
+        <c:crossAx val="-2118373112"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4303,7 +4311,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2136513240"/>
+        <c:axId val="-2118373112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4319,7 +4327,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="-2065148184"/>
+        <c:crossAx val="-2118817192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4379,7 +4387,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -4511,6 +4518,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -4542,112 +4550,112 @@
                 <c:formatCode>mmm\-yy</c:formatCode>
                 <c:ptCount val="36"/>
                 <c:pt idx="0">
-                  <c:v>43482.0</c:v>
+                  <c:v>43493.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43513.0</c:v>
+                  <c:v>43524.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43541.0</c:v>
+                  <c:v>43552.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43572.0</c:v>
+                  <c:v>43583.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43602.0</c:v>
+                  <c:v>43613.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43633.0</c:v>
+                  <c:v>43644.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43663.0</c:v>
+                  <c:v>43674.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43694.0</c:v>
+                  <c:v>43705.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43725.0</c:v>
+                  <c:v>43736.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43755.0</c:v>
+                  <c:v>43766.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43786.0</c:v>
+                  <c:v>43797.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43816.0</c:v>
+                  <c:v>43827.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43847.0</c:v>
+                  <c:v>43858.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43878.0</c:v>
+                  <c:v>43889.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>43907.0</c:v>
+                  <c:v>43918.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>43938.0</c:v>
+                  <c:v>43949.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>43968.0</c:v>
+                  <c:v>43979.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>43999.0</c:v>
+                  <c:v>44010.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>44029.0</c:v>
+                  <c:v>44040.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>44060.0</c:v>
+                  <c:v>44071.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>44091.0</c:v>
+                  <c:v>44102.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>44121.0</c:v>
+                  <c:v>44132.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>44152.0</c:v>
+                  <c:v>44163.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>44182.0</c:v>
+                  <c:v>44193.0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>44213.0</c:v>
+                  <c:v>44224.0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>44244.0</c:v>
+                  <c:v>44255.0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>44272.0</c:v>
+                  <c:v>44283.0</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>44303.0</c:v>
+                  <c:v>44314.0</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>44333.0</c:v>
+                  <c:v>44344.0</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>44364.0</c:v>
+                  <c:v>44375.0</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>44394.0</c:v>
+                  <c:v>44405.0</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>44425.0</c:v>
+                  <c:v>44436.0</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>44456.0</c:v>
+                  <c:v>44467.0</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>44486.0</c:v>
+                  <c:v>44497.0</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>44517.0</c:v>
+                  <c:v>44528.0</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>44547.0</c:v>
+                  <c:v>44558.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4792,112 +4800,112 @@
                 <c:formatCode>mmm\-yy</c:formatCode>
                 <c:ptCount val="36"/>
                 <c:pt idx="0">
-                  <c:v>43482.0</c:v>
+                  <c:v>43493.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43513.0</c:v>
+                  <c:v>43524.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43541.0</c:v>
+                  <c:v>43552.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43572.0</c:v>
+                  <c:v>43583.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43602.0</c:v>
+                  <c:v>43613.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43633.0</c:v>
+                  <c:v>43644.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43663.0</c:v>
+                  <c:v>43674.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43694.0</c:v>
+                  <c:v>43705.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43725.0</c:v>
+                  <c:v>43736.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43755.0</c:v>
+                  <c:v>43766.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43786.0</c:v>
+                  <c:v>43797.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43816.0</c:v>
+                  <c:v>43827.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43847.0</c:v>
+                  <c:v>43858.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43878.0</c:v>
+                  <c:v>43889.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>43907.0</c:v>
+                  <c:v>43918.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>43938.0</c:v>
+                  <c:v>43949.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>43968.0</c:v>
+                  <c:v>43979.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>43999.0</c:v>
+                  <c:v>44010.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>44029.0</c:v>
+                  <c:v>44040.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>44060.0</c:v>
+                  <c:v>44071.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>44091.0</c:v>
+                  <c:v>44102.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>44121.0</c:v>
+                  <c:v>44132.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>44152.0</c:v>
+                  <c:v>44163.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>44182.0</c:v>
+                  <c:v>44193.0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>44213.0</c:v>
+                  <c:v>44224.0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>44244.0</c:v>
+                  <c:v>44255.0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>44272.0</c:v>
+                  <c:v>44283.0</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>44303.0</c:v>
+                  <c:v>44314.0</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>44333.0</c:v>
+                  <c:v>44344.0</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>44364.0</c:v>
+                  <c:v>44375.0</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>44394.0</c:v>
+                  <c:v>44405.0</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>44425.0</c:v>
+                  <c:v>44436.0</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>44456.0</c:v>
+                  <c:v>44467.0</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>44486.0</c:v>
+                  <c:v>44497.0</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>44517.0</c:v>
+                  <c:v>44528.0</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>44547.0</c:v>
+                  <c:v>44558.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5030,8 +5038,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-2073550312"/>
-        <c:axId val="-2076283880"/>
+        <c:axId val="-2113556792"/>
+        <c:axId val="-2113460488"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -5060,112 +5068,112 @@
                 <c:formatCode>mmm\-yy</c:formatCode>
                 <c:ptCount val="36"/>
                 <c:pt idx="0">
-                  <c:v>43482.0</c:v>
+                  <c:v>43493.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43513.0</c:v>
+                  <c:v>43524.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43541.0</c:v>
+                  <c:v>43552.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43572.0</c:v>
+                  <c:v>43583.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43602.0</c:v>
+                  <c:v>43613.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43633.0</c:v>
+                  <c:v>43644.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43663.0</c:v>
+                  <c:v>43674.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43694.0</c:v>
+                  <c:v>43705.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43725.0</c:v>
+                  <c:v>43736.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43755.0</c:v>
+                  <c:v>43766.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43786.0</c:v>
+                  <c:v>43797.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43816.0</c:v>
+                  <c:v>43827.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43847.0</c:v>
+                  <c:v>43858.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43878.0</c:v>
+                  <c:v>43889.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>43907.0</c:v>
+                  <c:v>43918.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>43938.0</c:v>
+                  <c:v>43949.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>43968.0</c:v>
+                  <c:v>43979.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>43999.0</c:v>
+                  <c:v>44010.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>44029.0</c:v>
+                  <c:v>44040.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>44060.0</c:v>
+                  <c:v>44071.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>44091.0</c:v>
+                  <c:v>44102.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>44121.0</c:v>
+                  <c:v>44132.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>44152.0</c:v>
+                  <c:v>44163.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>44182.0</c:v>
+                  <c:v>44193.0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>44213.0</c:v>
+                  <c:v>44224.0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>44244.0</c:v>
+                  <c:v>44255.0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>44272.0</c:v>
+                  <c:v>44283.0</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>44303.0</c:v>
+                  <c:v>44314.0</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>44333.0</c:v>
+                  <c:v>44344.0</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>44364.0</c:v>
+                  <c:v>44375.0</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>44394.0</c:v>
+                  <c:v>44405.0</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>44425.0</c:v>
+                  <c:v>44436.0</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>44456.0</c:v>
+                  <c:v>44467.0</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>44486.0</c:v>
+                  <c:v>44497.0</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>44517.0</c:v>
+                  <c:v>44528.0</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>44547.0</c:v>
+                  <c:v>44558.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5299,11 +5307,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2073237896"/>
-        <c:axId val="-2076933416"/>
+        <c:axId val="-2118146568"/>
+        <c:axId val="-2110410728"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="-2073237896"/>
+        <c:axId val="-2118146568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5313,14 +5321,14 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2076933416"/>
+        <c:crossAx val="-2110410728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="months"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-2076933416"/>
+        <c:axId val="-2110410728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5336,12 +5344,12 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="-2073237896"/>
+        <c:crossAx val="-2118146568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2076283880"/>
+        <c:axId val="-2113460488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5351,12 +5359,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2073550312"/>
+        <c:crossAx val="-2113556792"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:dateAx>
-        <c:axId val="-2073550312"/>
+        <c:axId val="-2113556792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5366,7 +5374,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2076283880"/>
+        <c:crossAx val="-2113460488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -5375,6 +5383,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -6090,8 +6099,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2138188600"/>
-        <c:axId val="-2065258936"/>
+        <c:axId val="-2110357096"/>
+        <c:axId val="-2113701048"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -6430,11 +6439,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2136613864"/>
-        <c:axId val="-2065720504"/>
+        <c:axId val="-2118168840"/>
+        <c:axId val="-2113335368"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="2138188600"/>
+        <c:axId val="-2110357096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6444,14 +6453,14 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2065258936"/>
+        <c:crossAx val="-2113701048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="months"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-2065258936"/>
+        <c:axId val="-2113701048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6467,12 +6476,12 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="2138188600"/>
+        <c:crossAx val="-2110357096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2065720504"/>
+        <c:axId val="-2113335368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6482,12 +6491,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2136613864"/>
+        <c:crossAx val="-2118168840"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:dateAx>
-        <c:axId val="2136613864"/>
+        <c:axId val="-2118168840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6497,7 +6506,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2065720504"/>
+        <c:crossAx val="-2113335368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -6536,9 +6545,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>7073900</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:colOff>6997700</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -6548,7 +6557,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="330200" y="114300"/>
-          <a:ext cx="7188200" cy="2895600"/>
+          <a:ext cx="7112000" cy="3289300"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6608,6 +6617,50 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>7315200</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>101601</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>13169900</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>127653</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2" descr="runway_demo.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7759700" y="101601"/>
+          <a:ext cx="5854700" cy="3302652"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -8166,22 +8219,22 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:B90"/>
+  <dimension ref="B2:B91"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="17" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="5.83203125" style="60" customWidth="1"/>
-    <col min="2" max="2" width="192" style="60" customWidth="1"/>
+    <col min="2" max="2" width="173.83203125" style="60" customWidth="1"/>
     <col min="3" max="16384" width="10.83203125" style="60"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:2" ht="20">
       <c r="B2" s="102" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
     <row r="3" spans="2:2">
@@ -8194,7 +8247,7 @@
     </row>
     <row r="5" spans="2:2">
       <c r="B5" s="30" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="6" spans="2:2">
@@ -8217,374 +8270,379 @@
     </row>
     <row r="10" spans="2:2">
       <c r="B10" s="105" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="11" spans="2:2">
       <c r="B11" s="105" t="s">
-        <v>305</v>
+        <v>327</v>
       </c>
     </row>
     <row r="12" spans="2:2">
       <c r="B12" s="105" t="s">
-        <v>304</v>
+        <v>325</v>
       </c>
     </row>
     <row r="13" spans="2:2">
-      <c r="B13" s="103" t="s">
-        <v>228</v>
+      <c r="B13" s="105" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="14" spans="2:2">
-      <c r="B14" s="106" t="s">
-        <v>229</v>
+      <c r="B14" s="103" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="15" spans="2:2">
-      <c r="B15" s="30"/>
+      <c r="B15" s="106" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="16" spans="2:2">
       <c r="B16" s="30"/>
     </row>
     <row r="17" spans="2:2">
-      <c r="B17" s="62" t="s">
+      <c r="B17" s="30"/>
+    </row>
+    <row r="18" spans="2:2">
+      <c r="B18" s="62" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="2:2" ht="34">
-      <c r="B18" s="61" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2">
-      <c r="B19" s="61"/>
+    <row r="19" spans="2:2" ht="34">
+      <c r="B19" s="61" t="s">
+        <v>216</v>
+      </c>
     </row>
     <row r="20" spans="2:2">
-      <c r="B20" s="62" t="s">
+      <c r="B20" s="61"/>
+    </row>
+    <row r="21" spans="2:2">
+      <c r="B21" s="62" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="2:2" ht="34">
-      <c r="B21" s="61" t="s">
+    <row r="22" spans="2:2" ht="34">
+      <c r="B22" s="61" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="22" spans="2:2">
-      <c r="B22" s="61"/>
     </row>
     <row r="23" spans="2:2">
-      <c r="B23" s="62" t="s">
-        <v>89</v>
-      </c>
+      <c r="B23" s="61"/>
     </row>
     <row r="24" spans="2:2">
-      <c r="B24" s="61" t="s">
-        <v>306</v>
+      <c r="B24" s="62" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="25" spans="2:2">
-      <c r="B25" s="61"/>
+      <c r="B25" s="61" t="s">
+        <v>302</v>
+      </c>
     </row>
     <row r="26" spans="2:2">
-      <c r="B26" s="62" t="s">
-        <v>47</v>
-      </c>
+      <c r="B26" s="61"/>
     </row>
     <row r="27" spans="2:2">
-      <c r="B27" s="61" t="s">
+      <c r="B27" s="62" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2">
+      <c r="B28" s="61" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="28" spans="2:2" ht="34">
-      <c r="B28" s="61" t="s">
+    <row r="29" spans="2:2" ht="34">
+      <c r="B29" s="61" t="s">
         <v>91</v>
-      </c>
-    </row>
-    <row r="29" spans="2:2">
-      <c r="B29" s="61" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="30" spans="2:2">
-      <c r="B30" s="62" t="s">
-        <v>92</v>
+      <c r="B30" s="61" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="31" spans="2:2">
-      <c r="B31" s="61" t="s">
-        <v>93</v>
+      <c r="B31" s="62" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="32" spans="2:2">
       <c r="B32" s="61" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="33" spans="2:2">
       <c r="B33" s="61" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2">
+      <c r="B34" s="61" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="34" spans="2:2" ht="34">
-      <c r="B34" s="61" t="s">
+    <row r="35" spans="2:2" ht="34">
+      <c r="B35" s="61" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="35" spans="2:2">
-      <c r="B35" s="61" t="s">
+    <row r="36" spans="2:2">
+      <c r="B36" s="61" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="36" spans="2:2" ht="34">
-      <c r="B36" s="61" t="s">
+    <row r="37" spans="2:2" ht="51">
+      <c r="B37" s="61" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="37" spans="2:2">
-      <c r="B37" s="61"/>
     </row>
     <row r="38" spans="2:2">
-      <c r="B38" s="62" t="s">
-        <v>48</v>
-      </c>
+      <c r="B38" s="61"/>
     </row>
     <row r="39" spans="2:2">
-      <c r="B39" s="61" t="s">
+      <c r="B39" s="62" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2" ht="34">
+      <c r="B40" s="61" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="40" spans="2:2">
-      <c r="B40" s="61"/>
     </row>
     <row r="41" spans="2:2">
-      <c r="B41" s="93" t="s">
-        <v>176</v>
-      </c>
+      <c r="B41" s="61"/>
     </row>
     <row r="42" spans="2:2">
-      <c r="B42" s="94" t="s">
-        <v>177</v>
+      <c r="B42" s="93" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="43" spans="2:2">
       <c r="B43" s="94" t="s">
-        <v>50</v>
+        <v>177</v>
       </c>
     </row>
     <row r="44" spans="2:2">
       <c r="B44" s="94" t="s">
-        <v>178</v>
+        <v>50</v>
       </c>
     </row>
     <row r="45" spans="2:2">
       <c r="B45" s="94" t="s">
-        <v>156</v>
+        <v>178</v>
       </c>
     </row>
     <row r="46" spans="2:2">
-      <c r="B46" s="95"/>
+      <c r="B46" s="94" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="47" spans="2:2">
-      <c r="B47" s="97" t="s">
-        <v>179</v>
-      </c>
+      <c r="B47" s="95"/>
     </row>
     <row r="48" spans="2:2">
-      <c r="B48" s="97"/>
+      <c r="B48" s="97" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="49" spans="2:2">
-      <c r="B49" s="98" t="s">
+      <c r="B49" s="97"/>
+    </row>
+    <row r="50" spans="2:2">
+      <c r="B50" s="98" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="50" spans="2:2" ht="34">
-      <c r="B50" s="30" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="51" spans="2:2">
-      <c r="B51" s="30"/>
+    <row r="51" spans="2:2" ht="51">
+      <c r="B51" s="30" t="s">
+        <v>208</v>
+      </c>
     </row>
     <row r="52" spans="2:2">
-      <c r="B52" s="98" t="s">
+      <c r="B52" s="30"/>
+    </row>
+    <row r="53" spans="2:2">
+      <c r="B53" s="98" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="53" spans="2:2" ht="68">
-      <c r="B53" s="30" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="54" spans="2:2">
-      <c r="B54" s="30"/>
+    <row r="54" spans="2:2" ht="85">
+      <c r="B54" s="30" t="s">
+        <v>209</v>
+      </c>
     </row>
     <row r="55" spans="2:2">
-      <c r="B55" s="98" t="s">
+      <c r="B55" s="30"/>
+    </row>
+    <row r="56" spans="2:2">
+      <c r="B56" s="98" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="56" spans="2:2" ht="51">
-      <c r="B56" s="30" t="s">
-        <v>183</v>
+    <row r="57" spans="2:2" ht="85">
+      <c r="B57" s="30" t="s">
+        <v>326</v>
       </c>
     </row>
-    <row r="57" spans="2:2" ht="34">
-      <c r="B57" s="30" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="58" spans="2:2">
-      <c r="B58" s="30"/>
+    <row r="58" spans="2:2" ht="34">
+      <c r="B58" s="30" t="s">
+        <v>330</v>
+      </c>
     </row>
     <row r="59" spans="2:2">
-      <c r="B59" s="98" t="s">
-        <v>185</v>
-      </c>
+      <c r="B59" s="30"/>
     </row>
-    <row r="60" spans="2:2" ht="68">
-      <c r="B60" s="30" t="s">
-        <v>186</v>
+    <row r="60" spans="2:2">
+      <c r="B60" s="98" t="s">
+        <v>183</v>
       </c>
     </row>
-    <row r="61" spans="2:2">
+    <row r="61" spans="2:2" ht="34">
       <c r="B61" s="30" t="s">
-        <v>187</v>
+        <v>329</v>
       </c>
     </row>
-    <row r="62" spans="2:2">
-      <c r="B62" s="30"/>
+    <row r="62" spans="2:2" ht="34">
+      <c r="B62" s="30" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="63" spans="2:2">
-      <c r="B63" s="98" t="s">
-        <v>188</v>
-      </c>
+      <c r="B63" s="30"/>
     </row>
-    <row r="64" spans="2:2" ht="51">
-      <c r="B64" s="30" t="s">
-        <v>189</v>
+    <row r="64" spans="2:2">
+      <c r="B64" s="98" t="s">
+        <v>185</v>
       </c>
     </row>
-    <row r="65" spans="2:2" ht="68">
+    <row r="65" spans="2:2" ht="51">
       <c r="B65" s="30" t="s">
-        <v>213</v>
+        <v>186</v>
       </c>
     </row>
-    <row r="66" spans="2:2" ht="51">
+    <row r="66" spans="2:2" ht="68">
       <c r="B66" s="30" t="s">
-        <v>190</v>
+        <v>210</v>
       </c>
     </row>
-    <row r="67" spans="2:2" ht="34">
+    <row r="67" spans="2:2" ht="51">
       <c r="B67" s="30" t="s">
-        <v>215</v>
+        <v>187</v>
       </c>
     </row>
-    <row r="68" spans="2:2">
-      <c r="B68" s="30"/>
+    <row r="68" spans="2:2" ht="34">
+      <c r="B68" s="30" t="s">
+        <v>212</v>
+      </c>
     </row>
     <row r="69" spans="2:2">
-      <c r="B69" s="98" t="s">
-        <v>191</v>
-      </c>
+      <c r="B69" s="30"/>
     </row>
-    <row r="70" spans="2:2" ht="51">
-      <c r="B70" s="30" t="s">
-        <v>214</v>
+    <row r="70" spans="2:2">
+      <c r="B70" s="98" t="s">
+        <v>188</v>
       </c>
     </row>
-    <row r="71" spans="2:2">
-      <c r="B71" s="30"/>
+    <row r="71" spans="2:2" ht="51">
+      <c r="B71" s="30" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="72" spans="2:2">
-      <c r="B72" s="98" t="s">
-        <v>192</v>
-      </c>
+      <c r="B72" s="30"/>
     </row>
-    <row r="73" spans="2:2" ht="51">
-      <c r="B73" s="30" t="s">
-        <v>193</v>
+    <row r="73" spans="2:2">
+      <c r="B73" s="98" t="s">
+        <v>189</v>
       </c>
     </row>
-    <row r="74" spans="2:2">
-      <c r="B74" s="30"/>
+    <row r="74" spans="2:2" ht="51">
+      <c r="B74" s="30" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="75" spans="2:2">
-      <c r="B75" s="98" t="s">
-        <v>194</v>
-      </c>
+      <c r="B75" s="30"/>
     </row>
     <row r="76" spans="2:2">
-      <c r="B76" s="30" t="s">
-        <v>195</v>
+      <c r="B76" s="98" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="77" spans="2:2">
-      <c r="B77" s="30"/>
+      <c r="B77" s="30" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="78" spans="2:2">
-      <c r="B78" s="98" t="s">
-        <v>196</v>
-      </c>
+      <c r="B78" s="30"/>
     </row>
     <row r="79" spans="2:2">
-      <c r="B79" s="30" t="s">
-        <v>216</v>
+      <c r="B79" s="98" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="80" spans="2:2">
       <c r="B80" s="30" t="s">
-        <v>197</v>
+        <v>213</v>
       </c>
     </row>
     <row r="81" spans="2:2">
       <c r="B81" s="30" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
-    <row r="82" spans="2:2" ht="51">
+    <row r="82" spans="2:2">
       <c r="B82" s="30" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
-    <row r="83" spans="2:2">
-      <c r="B83" s="30"/>
+    <row r="83" spans="2:2" ht="51">
+      <c r="B83" s="30" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="84" spans="2:2">
-      <c r="B84" s="98" t="s">
-        <v>200</v>
-      </c>
+      <c r="B84" s="30"/>
     </row>
-    <row r="85" spans="2:2" ht="34">
-      <c r="B85" s="30" t="s">
-        <v>201</v>
+    <row r="85" spans="2:2">
+      <c r="B85" s="98" t="s">
+        <v>197</v>
       </c>
     </row>
-    <row r="86" spans="2:2">
-      <c r="B86" s="30"/>
+    <row r="86" spans="2:2" ht="34">
+      <c r="B86" s="30" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="87" spans="2:2">
-      <c r="B87" s="98" t="s">
-        <v>202</v>
-      </c>
+      <c r="B87" s="30"/>
     </row>
     <row r="88" spans="2:2">
-      <c r="B88" s="30" t="s">
-        <v>203</v>
+      <c r="B88" s="98" t="s">
+        <v>199</v>
       </c>
     </row>
-    <row r="89" spans="2:2" ht="34">
+    <row r="89" spans="2:2">
       <c r="B89" s="30" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="90" spans="2:2" ht="34">
       <c r="B90" s="30" t="s">
-        <v>205</v>
+        <v>201</v>
+      </c>
+    </row>
+    <row r="91" spans="2:2" ht="34">
+      <c r="B91" s="30" t="s">
+        <v>202</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B76" r:id="rId1"/>
+    <hyperlink ref="B77" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="63" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -8653,7 +8711,7 @@
     </row>
     <row r="15" spans="2:2" ht="20">
       <c r="B15" s="90" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
     </row>
     <row r="16" spans="2:2" ht="20">
@@ -8815,16 +8873,16 @@
         <v>160</v>
       </c>
       <c r="C7" s="96" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="66"/>
       <c r="B8" s="96" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C8" s="96" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -8851,7 +8909,7 @@
         <v>103</v>
       </c>
       <c r="C11" s="68" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -8860,7 +8918,7 @@
         <v>104</v>
       </c>
       <c r="C12" s="68" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -8982,13 +9040,13 @@
     </row>
     <row r="6" spans="2:8">
       <c r="B6" s="27" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D6" s="32" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="F6" s="95" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="7" spans="2:8">
@@ -9008,7 +9066,7 @@
       </c>
       <c r="D8" s="33">
         <f ca="1">TODAY()</f>
-        <v>43482</v>
+        <v>43493</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>32</v>
@@ -9052,13 +9110,13 @@
     </row>
     <row r="13" spans="2:8">
       <c r="B13" s="28" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="F13" s="26"/>
     </row>
     <row r="15" spans="2:8">
       <c r="B15" s="27" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C15" s="31" t="s">
         <v>24</v>
@@ -9067,13 +9125,13 @@
         <v>0</v>
       </c>
       <c r="F15" s="108" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="H15" s="35"/>
     </row>
     <row r="16" spans="2:8">
       <c r="B16" s="27" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C16" s="31" t="s">
         <v>24</v>
@@ -9082,7 +9140,7 @@
         <v>0</v>
       </c>
       <c r="F16" s="108" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="H16" s="35"/>
     </row>
@@ -9093,17 +9151,17 @@
     </row>
     <row r="19" spans="2:8">
       <c r="F19" s="133" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
     </row>
     <row r="20" spans="2:8">
       <c r="F20" s="134" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
     </row>
     <row r="21" spans="2:8" ht="34">
       <c r="F21" s="64" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
     </row>
     <row r="22" spans="2:8">
@@ -9111,7 +9169,7 @@
     </row>
     <row r="23" spans="2:8">
       <c r="F23" s="64" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
     </row>
     <row r="24" spans="2:8">
@@ -9119,22 +9177,22 @@
     </row>
     <row r="25" spans="2:8" ht="34">
       <c r="F25" s="64" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
     </row>
     <row r="26" spans="2:8">
       <c r="F26" s="64" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
     </row>
     <row r="27" spans="2:8" ht="34">
       <c r="F27" s="64" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
     </row>
     <row r="28" spans="2:8" ht="34">
       <c r="F28" s="64" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
     </row>
     <row r="29" spans="2:8">
@@ -9142,22 +9200,22 @@
     </row>
     <row r="30" spans="2:8">
       <c r="F30" s="133" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
     </row>
     <row r="31" spans="2:8">
       <c r="F31" s="134" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
     </row>
     <row r="32" spans="2:8" ht="68">
       <c r="F32" s="64" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
     </row>
     <row r="33" spans="6:6" ht="102">
       <c r="F33" s="64" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
     </row>
     <row r="34" spans="6:6">
@@ -9168,17 +9226,17 @@
     </row>
     <row r="36" spans="6:6">
       <c r="F36" s="133" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
     </row>
     <row r="37" spans="6:6">
       <c r="F37" s="134" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
     </row>
     <row r="38" spans="6:6">
       <c r="F38" s="30" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
     </row>
   </sheetData>
@@ -9197,9 +9255,9 @@
   <dimension ref="B2:AX150"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B2" sqref="B2"/>
-      <selection pane="bottomLeft" activeCell="C126" sqref="C126"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0"/>
@@ -9381,147 +9439,147 @@
       </c>
       <c r="C8" s="4">
         <f ca="1">'Get Started'!D8</f>
-        <v>43482</v>
+        <v>43493</v>
       </c>
       <c r="D8" s="4">
         <f ca="1">EDATE(C8,1)</f>
-        <v>43513</v>
+        <v>43524</v>
       </c>
       <c r="E8" s="4">
         <f t="shared" ref="E8:AL8" ca="1" si="1">EDATE(D8,1)</f>
-        <v>43541</v>
+        <v>43552</v>
       </c>
       <c r="F8" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>43572</v>
+        <v>43583</v>
       </c>
       <c r="G8" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>43602</v>
+        <v>43613</v>
       </c>
       <c r="H8" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>43633</v>
+        <v>43644</v>
       </c>
       <c r="I8" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>43663</v>
+        <v>43674</v>
       </c>
       <c r="J8" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>43694</v>
+        <v>43705</v>
       </c>
       <c r="K8" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>43725</v>
+        <v>43736</v>
       </c>
       <c r="L8" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>43755</v>
+        <v>43766</v>
       </c>
       <c r="M8" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>43786</v>
+        <v>43797</v>
       </c>
       <c r="N8" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>43816</v>
+        <v>43827</v>
       </c>
       <c r="O8" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>43847</v>
+        <v>43858</v>
       </c>
       <c r="P8" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>43878</v>
+        <v>43889</v>
       </c>
       <c r="Q8" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>43907</v>
+        <v>43918</v>
       </c>
       <c r="R8" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>43938</v>
+        <v>43949</v>
       </c>
       <c r="S8" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>43968</v>
+        <v>43979</v>
       </c>
       <c r="T8" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>43999</v>
+        <v>44010</v>
       </c>
       <c r="U8" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>44029</v>
+        <v>44040</v>
       </c>
       <c r="V8" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>44060</v>
+        <v>44071</v>
       </c>
       <c r="W8" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>44091</v>
+        <v>44102</v>
       </c>
       <c r="X8" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>44121</v>
+        <v>44132</v>
       </c>
       <c r="Y8" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>44152</v>
+        <v>44163</v>
       </c>
       <c r="Z8" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>44182</v>
+        <v>44193</v>
       </c>
       <c r="AA8" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>44213</v>
+        <v>44224</v>
       </c>
       <c r="AB8" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>44244</v>
+        <v>44255</v>
       </c>
       <c r="AC8" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>44272</v>
+        <v>44283</v>
       </c>
       <c r="AD8" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>44303</v>
+        <v>44314</v>
       </c>
       <c r="AE8" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>44333</v>
+        <v>44344</v>
       </c>
       <c r="AF8" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>44364</v>
+        <v>44375</v>
       </c>
       <c r="AG8" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>44394</v>
+        <v>44405</v>
       </c>
       <c r="AH8" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>44425</v>
+        <v>44436</v>
       </c>
       <c r="AI8" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>44456</v>
+        <v>44467</v>
       </c>
       <c r="AJ8" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>44486</v>
+        <v>44497</v>
       </c>
       <c r="AK8" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>44517</v>
+        <v>44528</v>
       </c>
       <c r="AL8" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>44547</v>
+        <v>44558</v>
       </c>
     </row>
     <row r="9" spans="2:38">
@@ -11182,7 +11240,7 @@
     </row>
     <row r="134" spans="2:50">
       <c r="B134" s="1" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="136" spans="2:50">
@@ -11766,7 +11824,7 @@
     </row>
     <row r="140" spans="2:50">
       <c r="B140" s="12" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="141" spans="2:50">
@@ -11774,7 +11832,7 @@
         <v>73</v>
       </c>
       <c r="C141" s="27" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="D141" s="2">
         <f>Forecast!G14</f>
@@ -11967,10 +12025,10 @@
     </row>
     <row r="142" spans="2:50">
       <c r="B142" s="129" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="C142" s="27" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="D142" s="36">
         <v>0</v>
@@ -12116,10 +12174,10 @@
     </row>
     <row r="143" spans="2:50">
       <c r="B143" s="129" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="C143" s="27" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="D143" s="36">
         <v>0</v>
@@ -12265,7 +12323,7 @@
     </row>
     <row r="145" spans="2:50">
       <c r="B145" s="12" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
     </row>
     <row r="146" spans="2:50">
@@ -12273,7 +12331,7 @@
         <v>73</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="D146" s="2">
         <f>INDEX(D141:D143,MATCH($B146,$B141:$B143,0))</f>
@@ -12466,10 +12524,10 @@
     </row>
     <row r="147" spans="2:50" s="7" customFormat="1">
       <c r="B147" s="7" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="C147" s="27" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="D147" s="128">
         <f ca="1">1-Forecast!G130</f>
@@ -12662,10 +12720,10 @@
     </row>
     <row r="148" spans="2:50" s="7" customFormat="1">
       <c r="B148" s="7" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="C148" s="27" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="D148" s="7">
         <f>Forecast!G81</f>
@@ -12884,10 +12942,10 @@
       <selection activeCell="J7" sqref="J7:J50"/>
       <selection pane="topRight" activeCell="J7" sqref="J7:J50"/>
       <selection pane="bottomLeft" activeCell="J7" sqref="J7:J50"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="BU3" sqref="BU3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="17" outlineLevelRow="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="17" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="3.83203125" style="26" customWidth="1"/>
     <col min="2" max="2" width="33.6640625" style="27" customWidth="1"/>
@@ -12895,9 +12953,11 @@
     <col min="4" max="4" width="16.6640625" style="27" customWidth="1"/>
     <col min="5" max="5" width="21" style="27" customWidth="1"/>
     <col min="6" max="6" width="14.83203125" style="27" customWidth="1"/>
-    <col min="7" max="53" width="14.83203125" style="26" customWidth="1"/>
-    <col min="54" max="71" width="12.6640625" style="26" customWidth="1"/>
-    <col min="72" max="75" width="15.1640625" style="26" customWidth="1"/>
+    <col min="7" max="53" width="14.83203125" style="26" customWidth="1" outlineLevel="1"/>
+    <col min="54" max="54" width="12.6640625" style="26" customWidth="1"/>
+    <col min="55" max="70" width="12.6640625" style="26" customWidth="1" outlineLevel="1"/>
+    <col min="71" max="71" width="12.6640625" style="26" customWidth="1"/>
+    <col min="72" max="75" width="15.1640625" style="26" customWidth="1" outlineLevel="1"/>
     <col min="76" max="16384" width="10.83203125" style="26"/>
   </cols>
   <sheetData>
@@ -15519,7 +15579,7 @@
     </row>
     <row r="14" spans="2:75" s="74" customFormat="1">
       <c r="B14" s="74" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="C14" s="81" t="str">
         <f>'Get Started'!$D$7</f>
@@ -27025,14 +27085,14 @@
     </row>
     <row r="60" spans="2:75" s="74" customFormat="1">
       <c r="B60" s="78" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="C60" s="75"/>
       <c r="D60" s="100" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E60" s="100" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="BC60" s="76"/>
       <c r="BD60" s="76"/>
@@ -27057,7 +27117,7 @@
     </row>
     <row r="61" spans="2:75" s="74" customFormat="1">
       <c r="B61" s="79" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C61" s="81" t="str">
         <f>'Get Started'!$D$7</f>
@@ -27072,7 +27132,7 @@
         <v>43861</v>
       </c>
       <c r="F61" s="74" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="G61" s="74">
         <f t="shared" ref="G61:P63" ca="1" si="244">IF(AND(G$5&lt;=$E61,G$5&gt;=$D61),G$50,0)</f>
@@ -27345,7 +27405,7 @@
     </row>
     <row r="62" spans="2:75" s="74" customFormat="1">
       <c r="B62" s="79" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C62" s="81" t="str">
         <f>'Get Started'!$D$7</f>
@@ -27360,7 +27420,7 @@
         <v>44255</v>
       </c>
       <c r="F62" s="74" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="G62" s="74">
         <f t="shared" ca="1" si="244"/>
@@ -27633,7 +27693,7 @@
     </row>
     <row r="63" spans="2:75" s="74" customFormat="1">
       <c r="B63" s="79" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C63" s="81" t="str">
         <f>'Get Started'!$D$7</f>
@@ -27648,7 +27708,7 @@
         <v>44895</v>
       </c>
       <c r="F63" s="74" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="G63" s="74">
         <f t="shared" ca="1" si="244"/>
@@ -29966,7 +30026,7 @@
     </row>
     <row r="77" spans="2:75" s="74" customFormat="1">
       <c r="B77" s="74" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="C77" s="75" t="str">
         <f>'Get Started'!$D$7</f>
@@ -30958,7 +31018,7 @@
         <v>$</v>
       </c>
       <c r="D83" s="74" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="G83" s="74">
         <f>MIN(G81:BA81)</f>
@@ -33427,22 +33487,22 @@
     </row>
     <row r="100" spans="1:76" s="50" customFormat="1">
       <c r="B100" s="110" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="D100" s="50" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="101" spans="1:76" s="50" customFormat="1" outlineLevel="1"/>
     <row r="102" spans="1:76" s="50" customFormat="1" outlineLevel="1">
       <c r="B102" s="50" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C102" s="111" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D102" s="50" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="G102" s="32">
         <v>0</v>
@@ -33617,7 +33677,7 @@
         <v>$</v>
       </c>
       <c r="D103" s="113" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="F103" s="50"/>
       <c r="G103" s="115">
@@ -33902,7 +33962,7 @@
         <v>$</v>
       </c>
       <c r="D104" s="113" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="F104" s="116">
         <v>0</v>
@@ -34216,7 +34276,7 @@
     <row r="106" spans="1:76" s="114" customFormat="1" outlineLevel="1">
       <c r="A106" s="112"/>
       <c r="B106" s="58" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C106" s="31"/>
       <c r="D106" s="113"/>
@@ -34261,7 +34321,7 @@
         <v>$</v>
       </c>
       <c r="D107" s="113" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="F107" s="115"/>
       <c r="G107" s="115">
@@ -34546,7 +34606,7 @@
         <v>$</v>
       </c>
       <c r="D108" s="113" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="F108" s="115"/>
       <c r="G108" s="32">
@@ -34784,7 +34844,7 @@
         <v>$</v>
       </c>
       <c r="D109" s="113" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="F109" s="115"/>
       <c r="G109" s="130">
@@ -35069,7 +35129,7 @@
         <v>$</v>
       </c>
       <c r="D110" s="113" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="F110" s="115"/>
       <c r="G110" s="115">
@@ -35346,13 +35406,13 @@
     <row r="111" spans="1:76" s="114" customFormat="1" outlineLevel="1">
       <c r="A111" s="112"/>
       <c r="B111" s="50" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C111" s="31" t="s">
         <v>24</v>
       </c>
       <c r="D111" s="113" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="F111" s="115"/>
       <c r="G111" s="117">
@@ -35575,7 +35635,7 @@
         <v>$</v>
       </c>
       <c r="D112" s="113" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="F112" s="115"/>
       <c r="G112" s="32">
@@ -35790,13 +35850,13 @@
     <row r="113" spans="1:76" s="114" customFormat="1" outlineLevel="1">
       <c r="A113" s="112"/>
       <c r="B113" s="50" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C113" s="31" t="s">
         <v>24</v>
       </c>
       <c r="D113" s="113" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="F113" s="115"/>
       <c r="G113" s="117">
@@ -36019,7 +36079,7 @@
         <v>$</v>
       </c>
       <c r="D114" s="113" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="F114" s="115"/>
       <c r="G114" s="115">
@@ -36303,7 +36363,7 @@
         <v>$</v>
       </c>
       <c r="D115" s="113" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="F115" s="115"/>
       <c r="G115" s="115">
@@ -36579,14 +36639,14 @@
     <row r="116" spans="1:76" s="114" customFormat="1" outlineLevel="1">
       <c r="A116" s="112"/>
       <c r="B116" s="50" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="C116" s="31" t="str">
         <f>'Get Started'!$D$7</f>
         <v>$</v>
       </c>
       <c r="D116" s="113" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="F116" s="115"/>
       <c r="G116" s="118">
@@ -36835,7 +36895,7 @@
     <row r="118" spans="1:76" s="114" customFormat="1" outlineLevel="1">
       <c r="A118" s="112"/>
       <c r="B118" s="58" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C118" s="31"/>
       <c r="D118" s="113"/>
@@ -36891,13 +36951,13 @@
     <row r="119" spans="1:76" s="114" customFormat="1" outlineLevel="1">
       <c r="A119" s="112"/>
       <c r="B119" s="50" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C119" s="119" t="s">
         <v>24</v>
       </c>
       <c r="D119" s="113" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="G119" s="117">
         <f>IF(G107&lt;&gt;0,'Get Started'!$D15,0)</f>
@@ -37091,14 +37151,14 @@
     <row r="120" spans="1:76" s="114" customFormat="1" outlineLevel="1">
       <c r="A120" s="112"/>
       <c r="B120" s="50" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C120" s="31" t="str">
         <f>'Get Started'!$D$7</f>
         <v>$</v>
       </c>
       <c r="D120" s="113" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="G120" s="115">
         <f t="shared" ref="G120:BA120" si="329">MAX(0,G121-G103)</f>
@@ -37292,14 +37352,14 @@
     <row r="121" spans="1:76" s="114" customFormat="1" outlineLevel="1">
       <c r="A121" s="112"/>
       <c r="B121" s="50" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C121" s="31" t="str">
         <f>'Get Started'!$D$7</f>
         <v>$</v>
       </c>
       <c r="D121" s="113" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="G121" s="120">
         <f t="shared" ref="G121:BA121" si="330">IFERROR(G103/G119,0)</f>
@@ -37493,13 +37553,13 @@
     <row r="122" spans="1:76" s="114" customFormat="1" outlineLevel="1">
       <c r="A122" s="112"/>
       <c r="B122" s="50" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C122" s="112" t="s">
         <v>66</v>
       </c>
       <c r="D122" s="113" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="G122" s="32">
         <v>10000000</v>
@@ -37692,13 +37752,13 @@
     <row r="123" spans="1:76" s="114" customFormat="1" outlineLevel="1">
       <c r="A123" s="112"/>
       <c r="B123" s="50" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C123" s="112" t="s">
         <v>66</v>
       </c>
       <c r="D123" s="113" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="G123" s="120">
         <f t="shared" ref="G123:BA123" ca="1" si="332">IFERROR(G103/G127,0)+IFERROR(G114/G116,0)</f>
@@ -37973,13 +38033,13 @@
     <row r="124" spans="1:76" s="114" customFormat="1" outlineLevel="1">
       <c r="A124" s="112"/>
       <c r="B124" s="50" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C124" s="112" t="s">
         <v>24</v>
       </c>
       <c r="D124" s="113" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="G124" s="117">
         <f>IF(G107&lt;&gt;0,'Get Started'!$D16,0)</f>
@@ -38173,13 +38233,13 @@
     <row r="125" spans="1:76" s="114" customFormat="1" outlineLevel="1">
       <c r="A125" s="112"/>
       <c r="B125" s="50" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C125" s="112" t="s">
         <v>66</v>
       </c>
       <c r="D125" s="113" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="G125" s="120">
         <f t="shared" ref="G125:BA125" ca="1" si="334">ROUND(G126-G122-G123,5)</f>
@@ -38454,13 +38514,13 @@
     <row r="126" spans="1:76" s="114" customFormat="1" outlineLevel="1">
       <c r="A126" s="112"/>
       <c r="B126" s="50" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="C126" s="112" t="s">
         <v>66</v>
       </c>
       <c r="D126" s="121" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="G126" s="120">
         <f t="shared" ref="G126:BA126" ca="1" si="337">IFERROR((G122+G123)/(1-G124),0)</f>
@@ -38735,14 +38795,14 @@
     <row r="127" spans="1:76" s="114" customFormat="1" outlineLevel="1">
       <c r="A127" s="112"/>
       <c r="B127" s="50" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C127" s="31" t="str">
         <f>'Get Started'!$D$7</f>
         <v>$</v>
       </c>
       <c r="D127" s="113" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="G127" s="122">
         <f t="shared" ref="G127:BA127" si="338">G120/G122</f>
@@ -38936,14 +38996,14 @@
     <row r="128" spans="1:76" s="114" customFormat="1" outlineLevel="1">
       <c r="A128" s="112"/>
       <c r="B128" s="50" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="C128" s="31" t="str">
         <f>'Get Started'!$D$7</f>
         <v>$</v>
       </c>
       <c r="D128" s="113" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F128" s="123">
         <v>0</v>
@@ -39140,13 +39200,13 @@
     <row r="129" spans="1:75" s="114" customFormat="1" outlineLevel="1">
       <c r="A129" s="112"/>
       <c r="B129" s="50" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="C129" s="112" t="s">
         <v>66</v>
       </c>
       <c r="D129" s="113" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="G129" s="120">
         <f ca="1">SUM($G123:G123)</f>
@@ -39421,13 +39481,13 @@
     <row r="130" spans="1:75" s="114" customFormat="1" outlineLevel="1">
       <c r="A130" s="112"/>
       <c r="B130" s="50" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="C130" s="112" t="s">
         <v>24</v>
       </c>
       <c r="D130" s="113" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="G130" s="124">
         <f t="shared" ref="G130:BA130" ca="1" si="341">IFERROR(G129/G126,0)</f>
@@ -39620,13 +39680,13 @@
     </row>
     <row r="131" spans="1:75" s="50" customFormat="1" outlineLevel="1">
       <c r="B131" s="50" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="C131" s="112" t="s">
         <v>66</v>
       </c>
       <c r="D131" s="50" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="G131" s="50">
         <f ca="1">IFERROR(G110/(G112/G122),0)+G126</f>
@@ -39903,18 +39963,18 @@
     </row>
     <row r="133" spans="1:75" s="50" customFormat="1" outlineLevel="1">
       <c r="B133" s="58" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="134" spans="1:75" s="50" customFormat="1" outlineLevel="1">
       <c r="B134" s="126" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="C134" s="112" t="s">
         <v>66</v>
       </c>
       <c r="D134" s="3" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="F134" s="50">
         <f>F139*F$136</f>
@@ -40191,7 +40251,7 @@
     </row>
     <row r="135" spans="1:75" s="50" customFormat="1" outlineLevel="1">
       <c r="B135" s="126" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="C135" s="112" t="s">
         <v>66</v>
@@ -40752,7 +40812,7 @@
     <row r="137" spans="1:75" s="50" customFormat="1" outlineLevel="1"/>
     <row r="138" spans="1:75" s="50" customFormat="1" outlineLevel="1">
       <c r="B138" s="58" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="139" spans="1:75" s="50" customFormat="1" outlineLevel="1">
@@ -41602,10 +41662,10 @@
     <row r="142" spans="1:75" s="50" customFormat="1" outlineLevel="1"/>
     <row r="143" spans="1:75" s="50" customFormat="1" outlineLevel="1">
       <c r="B143" s="50" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="D143" s="50" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="144" spans="1:75" s="50" customFormat="1" outlineLevel="1">
@@ -42461,10 +42521,10 @@
         <v>$ Invested</v>
       </c>
       <c r="F148" s="50" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="G148" s="50" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="J148" s="125"/>
       <c r="T148" s="24"/>
@@ -43102,11 +43162,11 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:B16"/>
+  <dimension ref="B2:B17"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0"/>
@@ -43124,7 +43184,7 @@
     <row r="3" spans="2:2" s="2" customFormat="1"/>
     <row r="4" spans="2:2" s="2" customFormat="1">
       <c r="B4" s="131" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
     </row>
     <row r="5" spans="2:2" s="2" customFormat="1">
@@ -43134,41 +43194,46 @@
     </row>
     <row r="6" spans="2:2" s="2" customFormat="1" ht="34">
       <c r="B6" s="85" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
     </row>
     <row r="7" spans="2:2" s="2" customFormat="1">
-      <c r="B7" s="85"/>
+      <c r="B7" s="85" t="s">
+        <v>328</v>
+      </c>
     </row>
     <row r="8" spans="2:2" s="2" customFormat="1">
-      <c r="B8" s="131" t="s">
+      <c r="B8" s="85"/>
+    </row>
+    <row r="9" spans="2:2" s="2" customFormat="1">
+      <c r="B9" s="131" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2" s="2" customFormat="1" ht="85">
+      <c r="B10" s="132" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2" s="2" customFormat="1"/>
+    <row r="12" spans="2:2">
+      <c r="B12" s="131" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="13" spans="2:2" ht="51">
+      <c r="B13" s="72" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="15" spans="2:2" ht="68">
+      <c r="B15" s="72" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="9" spans="2:2" s="2" customFormat="1" ht="85">
-      <c r="B9" s="132" t="s">
+    <row r="17" spans="2:2">
+      <c r="B17" s="7" t="s">
         <v>308</v>
-      </c>
-    </row>
-    <row r="10" spans="2:2" s="2" customFormat="1"/>
-    <row r="11" spans="2:2">
-      <c r="B11" s="131" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="12" spans="2:2" ht="51">
-      <c r="B12" s="72" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="14" spans="2:2" ht="68">
-      <c r="B14" s="72" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="16" spans="2:2">
-      <c r="B16" s="7" t="s">
-        <v>312</v>
       </c>
     </row>
   </sheetData>

</xml_diff>